<commit_message>
new plots added, modified some dataframes
</commit_message>
<xml_diff>
--- a/spotifystats/longframe.xlsx
+++ b/spotifystats/longframe.xlsx
@@ -604,7 +604,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.2630777999999999</v>
+        <v>0.2516977999999999</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.68926</v>
+        <v>0.6940400000000001</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.6163200000000001</v>
+        <v>0.6271400000000001</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -658,7 +658,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.001648378</v>
+        <v>0.001648606</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.17659</v>
+        <v>0.175328</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.58</v>
+        <v>0.6</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.087918</v>
+        <v>0.08866599999999998</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.4994799999999999</v>
+        <v>0.51018</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>

</xml_diff>